<commit_message>
Reconstruct missing data longitudinally
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
+++ b/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htetnaing/Development/htet_mces_bank_data/Experiment_Resulsts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5274285-EA06-0343-BE1B-9B3D76F29B13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B74BF5-C077-4105-8776-EEDAEBC6AA17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6100" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
   </bookViews>
   <sheets>
     <sheet name="first_10_records_no_NaN" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="19">
   <si>
     <t>eMFIS(I/E)</t>
   </si>
@@ -51,14 +51,50 @@
     <t>Denfis</t>
   </si>
   <si>
-    <t>Parallel_Ensemble_Anfis_Denfis</t>
+    <t>Failed_Banks_First_10_Records_no_NaN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Parallel_Ensemble_Anfis_Denfis_SA</t>
+  </si>
+  <si>
+    <t>Failed_Banks_Full_Records_no_NaN</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Parallel_Ensemble_Anfis_Denfis_BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target_Feature </t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>CAPADE</t>
+  </si>
+  <si>
+    <t>PLAQLY</t>
+  </si>
+  <si>
+    <t>Survived_Banks_Full_Records_no_NaN</t>
+  </si>
+  <si>
+    <t>Random-24%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,8 +118,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +153,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,12 +193,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,123 +523,907 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAED88D5-E873-5842-BA5A-48463FA2EFF5}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="21.09765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
         <v>0.72596362751813304</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.87247119004309204</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.49875543927129601</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0.906261284322321</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.22028893759366999</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>0.230542188231315</v>
+        <v>0.87247119004309204</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>0.84274048657332301</v>
+        <v>0.49875543927129601</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1">
-        <v>0.16158110816649199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.906261284322321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>0.299627150987539</v>
+        <v>0.22028893759366999</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4">
-        <v>0.25462939088374498</v>
+        <v>0.230542188231315</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4" s="4">
-        <v>0.891780721460393</v>
+        <v>0.84274048657332301</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4" s="1">
+        <v>0.16158110816649199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.299627150987539</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.25462939088374498</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.891780721460393</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.18985082789171401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="M9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="M10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="M11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="M12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="7">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="M16" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="M17" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="M18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="7">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="M22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="M23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="M24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="7">
+        <v>1</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="M28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="M29" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="M30" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="M31" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="7">
+        <v>1</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="M34" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="M35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="M36" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="1"/>
+      <c r="M37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="7">
+        <v>1</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="3"/>
+      <c r="M40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1"/>
+      <c r="M41" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K42" s="1"/>
+      <c r="M42" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="4"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" s="1"/>
+      <c r="M43" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add lateral prediction results for data reconstruction
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
+++ b/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
@@ -1,20 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B74BF5-C077-4105-8776-EEDAEBC6AA17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62867B63-0B24-4F0E-8288-5A4EE888B19D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
   </bookViews>
   <sheets>
     <sheet name="first_10_records_no_NaN" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">first_10_records_no_NaN!$A$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">first_10_records_no_NaN!$A$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">first_10_records_no_NaN!$B$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">first_10_records_no_NaN!$B$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">first_10_records_no_NaN!$B$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">first_10_records_no_NaN!$B$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">first_10_records_no_NaN!$A$3</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">first_10_records_no_NaN!$A$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">first_10_records_no_NaN!$A$5</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">first_10_records_no_NaN!$B$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">first_10_records_no_NaN!$B$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">first_10_records_no_NaN!$B$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">first_10_records_no_NaN!$A$5</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">first_10_records_no_NaN!$B$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">first_10_records_no_NaN!$B$2:$K$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">first_10_records_no_NaN!$B$3:$K$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">first_10_records_no_NaN!$B$4:$K$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">first_10_records_no_NaN!$B$5:$K$5</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">first_10_records_no_NaN!$A$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">first_10_records_no_NaN!$A$4</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">first_10_records_no_NaN!$A$5</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="24">
   <si>
     <t>eMFIS(I/E)</t>
   </si>
@@ -87,7 +110,22 @@
     <t>Survived_Banks_Full_Records_no_NaN</t>
   </si>
   <si>
-    <t>Random-24%</t>
+    <t>80% - 8</t>
+  </si>
+  <si>
+    <t>20% - 2</t>
+  </si>
+  <si>
+    <t>100% - 2485</t>
+  </si>
+  <si>
+    <t>Random-24% : 596</t>
+  </si>
+  <si>
+    <t>100% - 49338</t>
+  </si>
+  <si>
+    <t>Random-24% : 11841</t>
   </si>
 </sst>
 </file>
@@ -193,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -209,6 +247,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,13 +577,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAED88D5-E873-5842-BA5A-48463FA2EFF5}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="21.09765625" customWidth="1"/>
+    <col min="10" max="10" width="16.69921875" customWidth="1"/>
+    <col min="11" max="11" width="21.09765625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="19.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -552,14 +606,14 @@
       <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="J1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="7">
-        <v>0.2</v>
+      <c r="L1" s="16" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -581,7 +635,6 @@
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3"/>
       <c r="L2" t="s">
         <v>7</v>
       </c>
@@ -673,7 +726,9 @@
         <v>0.18985082789171401</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="19"/>
+    </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>9</v>
@@ -692,14 +747,14 @@
       <c r="I8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="7">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6" t="s">
+      <c r="J8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -721,7 +776,6 @@
       <c r="J9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="3"/>
       <c r="M9" s="2" t="s">
         <v>12</v>
       </c>
@@ -730,76 +784,106 @@
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="18">
+        <v>0.45836492551288899</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>0.34812994580241802</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4">
+        <v>0.17015409128153799</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="K10" s="3">
+        <v>0.43763074378760197</v>
+      </c>
       <c r="M10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="1"/>
+      <c r="N10" s="2">
+        <v>0.50266194419489996</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="18">
+        <v>2.1179695246560999E-2</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>2.2861332959128001E-2</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4">
+        <v>2.9505892924164001E-2</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11" s="3">
+        <v>2.1704809110686001E-2</v>
+      </c>
       <c r="M11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="2">
+        <v>1.9982141780791999E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="18">
+        <v>3.3932805913490002E-2</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>3.5804006884850997E-2</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4">
+        <v>4.3443999281090002E-2</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="3">
+        <v>3.4464253361791999E-2</v>
+      </c>
       <c r="M12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="2">
+        <v>3.3301969215006E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -819,14 +903,14 @@
       <c r="I14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="7">
-        <v>1</v>
-      </c>
-      <c r="K14" s="6" t="s">
+      <c r="J14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -848,7 +932,6 @@
       <c r="J15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="3"/>
       <c r="M15" s="2" t="s">
         <v>12</v>
       </c>
@@ -857,75 +940,108 @@
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>0.89566832815596098</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>0.53349562698048703</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="18">
+        <v>9.1222709172605998E-2</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="3">
+        <v>0.85809483603975101</v>
+      </c>
       <c r="M16" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="2">
+        <v>0.93532286005874399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="18">
+        <v>1.1440623970544E-2</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>2.1852975295213999E-2</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4">
+        <v>2.8505395793206E-2</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="3">
+        <v>1.5228634444047E-2</v>
+      </c>
       <c r="M17" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="2">
+        <v>8.8315943172130006E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="18">
+        <v>1.6828972460948999E-2</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>3.2198880865703002E-2</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4">
+        <v>4.3877732629796003E-2</v>
+      </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="3">
+        <v>2.1617135293241E-2</v>
+      </c>
       <c r="M18" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18" s="2">
+        <v>1.3953602509804999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
@@ -943,17 +1059,17 @@
       <c r="I20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="7">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6" t="s">
+      <c r="J20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>3</v>
       </c>
@@ -972,85 +1088,119 @@
       <c r="J21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="3"/>
       <c r="M21" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="18">
+        <v>0.59643867657364902</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4">
+        <v>0.27040698091867599</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4">
+        <v>-6.7656148034444002E-2</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="3">
+        <v>0.56140937931352897</v>
+      </c>
       <c r="M22" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22" s="2">
+        <v>0.67503228879446597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4">
+        <v>0.58100547363065802</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4">
+        <v>0.70171352215736504</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4">
+        <v>1.1720435895433701</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1">
+        <v>0.54126562508526199</v>
+      </c>
       <c r="M23" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23" s="2">
+        <v>0.39279606721249899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="18">
+        <v>2.0735806301248099</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4">
+        <v>2.48714459037526</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4">
+        <v>3.0727268536230299</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="1"/>
+      <c r="K24" s="3">
+        <v>2.1762585081452399</v>
+      </c>
       <c r="M24" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24" s="2">
+        <v>1.9724676830460599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="19"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
@@ -1068,17 +1218,17 @@
       <c r="I27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J27" s="7">
-        <v>1</v>
-      </c>
-      <c r="K27" s="6" t="s">
+      <c r="J27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>3</v>
       </c>
@@ -1097,84 +1247,116 @@
       <c r="J28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K28" s="3"/>
       <c r="M28" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="18">
+        <v>0.358330997834647</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>0.21538672035475201</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="4"/>
+      <c r="H29" s="4">
+        <v>3.2444982641652E-2</v>
+      </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="K29" s="3">
+        <v>0.33362699891365899</v>
+      </c>
       <c r="M29" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>0.51971269215604399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="18">
+        <v>1.9235129569053998E-2</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4">
+        <v>2.0358580179429001E-2</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4">
+        <v>2.4959530816991E-2</v>
+      </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="K30" s="3">
+        <v>1.9591486731495002E-2</v>
+      </c>
       <c r="M30" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>1.7413694326435001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="18">
+        <v>2.8053209439383001E-2</v>
+      </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4">
+        <v>2.9363460373889001E-2</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="4"/>
+      <c r="H31" s="4">
+        <v>3.605419317808E-2</v>
+      </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K31" s="1"/>
+      <c r="K31" s="3">
+        <v>2.8460198632512E-2</v>
+      </c>
       <c r="M31" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>2.6682724410981001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>17</v>
       </c>
@@ -1192,17 +1374,17 @@
       <c r="I33" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J33" s="7">
-        <v>1</v>
-      </c>
-      <c r="K33" s="6" t="s">
+      <c r="J33" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>3</v>
       </c>
@@ -1221,84 +1403,117 @@
       <c r="J34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K34" s="3"/>
       <c r="M34" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="18">
+        <v>0.74435617022431</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>0.54193239550653804</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4">
+        <v>4.0209674860595998E-2</v>
+      </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="1"/>
+      <c r="K35" s="3">
+        <v>0.697228063292752</v>
+      </c>
       <c r="M35" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N35">
+        <v>0.82127334097888305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="18">
+        <v>5.2469659843670004E-3</v>
+      </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4">
+        <v>8.2855601333939998E-3</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="4"/>
+      <c r="H36" s="4">
+        <v>7.5681135267770001E-3</v>
+      </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="1"/>
+      <c r="K36" s="3">
+        <v>6.4143787293820002E-3</v>
+      </c>
+      <c r="L36" s="17"/>
       <c r="M36" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N36">
+        <v>4.3608152155919996E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="18">
+        <v>8.7225664925190006E-3</v>
+      </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4">
+        <v>1.1762521138008001E-2</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="4"/>
+      <c r="H37" s="4">
+        <v>1.5032477077819999E-2</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K37" s="1"/>
+      <c r="K37" s="3">
+        <v>9.6387235549070006E-3</v>
+      </c>
       <c r="M37" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N37">
+        <v>7.739966554427E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>17</v>
       </c>
@@ -1316,17 +1531,17 @@
       <c r="I39" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J39" s="7">
-        <v>1</v>
-      </c>
-      <c r="K39" s="6" t="s">
+      <c r="J39" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>3</v>
       </c>
@@ -1345,81 +1560,113 @@
       <c r="J40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K40" s="3"/>
       <c r="M40" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="18">
+        <v>0.81627222708007896</v>
+      </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4">
+        <v>0.63978112370880202</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="4"/>
+      <c r="H41" s="4">
+        <v>4.4693870392302999E-2</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K41" s="1"/>
+      <c r="K41" s="3">
+        <v>0.78638016369599795</v>
+      </c>
       <c r="M41" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N41">
+        <v>0.86057123266455304</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="18">
+        <v>6.1839146302673002E-2</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4">
+        <v>6.5089191141605995E-2</v>
+      </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H42" s="4"/>
+      <c r="H42" s="4">
+        <v>0.10686449614843101</v>
+      </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K42" s="1"/>
+      <c r="K42" s="3">
+        <v>6.2419906672390002E-2</v>
+      </c>
       <c r="M42" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N42">
+        <v>5.5742461360743997E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="18">
+        <v>0.107416555706096</v>
+      </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4">
+        <v>0.14324006937289099</v>
+      </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H43" s="4"/>
+      <c r="H43" s="4">
+        <v>0.25369527619040499</v>
+      </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="1"/>
+      <c r="K43" s="3">
+        <v>0.117874784899597</v>
+      </c>
       <c r="M43" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="N43">
+        <v>9.7486536193885004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add experiment results for longitudinal construction
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
+++ b/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
@@ -8,36 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62867B63-0B24-4F0E-8288-5A4EE888B19D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CE116-25CF-4EAC-97A4-DA56D5281118}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
   </bookViews>
   <sheets>
-    <sheet name="first_10_records_no_NaN" sheetId="1" r:id="rId1"/>
+    <sheet name="first_10_records_full_lateral" sheetId="1" r:id="rId1"/>
+    <sheet name="last_3_records_full_vertical" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">first_10_records_no_NaN!$A$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">first_10_records_no_NaN!$A$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">first_10_records_no_NaN!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">first_10_records_no_NaN!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">first_10_records_no_NaN!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">first_10_records_no_NaN!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">first_10_records_no_NaN!$A$3</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">first_10_records_no_NaN!$A$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">first_10_records_no_NaN!$A$5</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">first_10_records_no_NaN!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">first_10_records_no_NaN!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">first_10_records_no_NaN!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">first_10_records_no_NaN!$A$5</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">first_10_records_no_NaN!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">first_10_records_no_NaN!$B$2:$K$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">first_10_records_no_NaN!$B$3:$K$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">first_10_records_no_NaN!$B$4:$K$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">first_10_records_no_NaN!$B$5:$K$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">first_10_records_no_NaN!$A$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">first_10_records_no_NaN!$A$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">first_10_records_no_NaN!$A$5</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -54,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="32">
   <si>
     <t>eMFIS(I/E)</t>
   </si>
@@ -127,12 +106,36 @@
   <si>
     <t>Random-24% : 11841</t>
   </si>
+  <si>
+    <t>Backward_Prediction</t>
+  </si>
+  <si>
+    <t>Forward Prediction</t>
+  </si>
+  <si>
+    <t>100% - 440</t>
+  </si>
+  <si>
+    <t>Random-24% :106</t>
+  </si>
+  <si>
+    <t>100% - 3271</t>
+  </si>
+  <si>
+    <t>Random-24% : 785</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Backward</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,8 +183,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +242,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -231,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,6 +303,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAED88D5-E873-5842-BA5A-48463FA2EFF5}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1673,4 +1724,2392 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71B7EED-AC09-4997-9EF3-1224B488CEBF}">
+  <dimension ref="A1:N77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" style="3"/>
+    <col min="10" max="10" width="16.69921875" customWidth="1"/>
+    <col min="11" max="11" width="21.09765625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="19.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.69481254169738804</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.60996284507335297</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>8.2026055506213003E-2</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.65985529632346496</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.72622902038709303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1.3647161408762E-2</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.4567556786340001E-2</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2.7439376498756E-2</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.4005143650075999E-2</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1.2161906369283999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2.2525171335086001E-2</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.4845346721758001E-2</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3.8946687478452001E-2</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2.3516958534254999E-2</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2.1627556161739E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0.50220655193284902</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.421722391205545</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24">
+        <v>0.104617196722817</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.51344721874439703</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.66531051026467702</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2.5001974754238002E-2</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.8245784740410999E-2</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3.6129425987647998E-2</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2.6132159782406E-2</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>2.1089386322075999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3.4251283982576E-2</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.6257835537842002E-2</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="4">
+        <v>4.8704008648731999E-2</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3.4524286602662997E-2</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="2">
+        <v>3.0617196507478999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.607117580723466</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.244786235894112</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>-5.1890733496519998E-3</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0.54478559615650302</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.74994858012927701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2.4122857304778198</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.6364637781231601</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4">
+        <v>3.2937137423709002</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>2.4693813606122501</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2.0262445142361498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="18">
+        <v>5.2710042781031303</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5.9440120903387701</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="4">
+        <v>6.8865699475227</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>5.5677850709058498</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="2">
+        <v>5.1056453440347802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="19"/>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.97333648617217094</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.97268333435183696</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.37552696557800003</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.97353290973206796</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.97597939880309104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5.0585177693840003E-3</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>5.1535939624740004E-3</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2.0201170793138001E-2</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="1">
+        <v>5.0544400544789998E-3</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" s="2">
+        <v>4.618171768085E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="4">
+        <v>7.6127248632249997E-3</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4">
+        <v>7.7161701336220002E-3</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="4">
+        <v>3.4005577762935002E-2</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="1">
+        <v>7.5896047708160002E-3</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="2">
+        <v>7.2322832204829999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="18">
+        <v>0.48360441899460899</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.425254589091484</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.142470668374616</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.47447533171511203</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0.55255087820020299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="4">
+        <v>2.629330426662E-3</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2.6781704441369999E-3</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="4">
+        <v>3.5774857596250001E-3</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2.625632403398E-3</v>
+      </c>
+      <c r="L30" s="17"/>
+      <c r="M30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" s="2">
+        <v>2.2936519597009999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="18">
+        <v>5.3195656392579999E-3</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="4">
+        <v>5.5339441240559997E-3</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="4">
+        <v>6.730079641898E-3</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" s="3">
+        <v>5.3304964412619997E-3</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" s="2">
+        <v>5.01719582054E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.78423777657081095</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="18">
+        <v>0.80255038514895005</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.21388685747402</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0.79988386235055298</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0.83024528113752705</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="4">
+        <v>3.3498570673979003E-2</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>3.3052735417153999E-2</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="4">
+        <v>6.9037789459864995E-2</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K36" s="1">
+        <v>3.2869279807694003E-2</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N36" s="2">
+        <v>2.9243352877829001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="4">
+        <v>5.7968142520474997E-2</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="18">
+        <v>5.5751094627019999E-2</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.106377839015161</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="3">
+        <v>5.5974819909055999E-2</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N37" s="2">
+        <v>5.2147560880313998E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="22"/>
+      <c r="K38" s="22"/>
+    </row>
+    <row r="39" spans="1:14" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="10"/>
+      <c r="I40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="18">
+        <v>0.864164651231076</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.83482332871085896</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.23664072723639801</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0.85576902229480001</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N42" s="2">
+        <v>0.88307062528189195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="18">
+        <v>1.0246652001194E-2</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1.1985796854428001E-2</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="4">
+        <v>1.9660754261543002E-2</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="3">
+        <v>1.1076635978866E-2</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N43" s="2">
+        <v>9.2222120670809992E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="18">
+        <v>1.4339525504621E-2</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1.7392168805881E-2</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="4">
+        <v>3.0253586184688E-2</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" s="3">
+        <v>1.514573004528E-2</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N44" s="2">
+        <v>1.3368222413911E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="18">
+        <v>0.52844073459788399</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0.29346157934358902</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4">
+        <v>-3.4865881429239E-2</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>0.50057868619458601</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N48" s="2">
+        <v>0.70572858024795904</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="18">
+        <v>1.7269844828825001E-2</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="4">
+        <v>1.8378573378521001E-2</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H49" s="4">
+        <v>2.5269520045205999E-2</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K49" s="3">
+        <v>1.7587268890391999E-2</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1.4225611702954E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="18">
+        <v>2.5561167111114998E-2</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2.8581611528096001E-2</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" s="4">
+        <v>4.4193845261584999E-2</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K50" s="3">
+        <v>2.6548186006718998E-2</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N50" s="2">
+        <v>2.3622818218097998E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="18">
+        <v>0.844379177287788</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4">
+        <v>0.77334069249852799</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H54" s="4">
+        <v>-0.10399366162814599</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0.83652032752707695</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N54" s="2">
+        <v>0.86343100010207396</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="18">
+        <v>0.17980206266523999</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0.22273719842943701</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H55" s="4">
+        <v>0.422576846097171</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0.19451810787250401</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N55" s="2">
+        <v>0.167212890471367</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="18">
+        <v>0.237000320009776</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0.28733366256116</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="4">
+        <v>0.78991127042911202</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0.24919175146257699</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N56" s="2">
+        <v>0.22446821539057099</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="19"/>
+      <c r="K58" s="19"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="10"/>
+      <c r="I59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K59" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="18">
+        <v>0.98374923020516503</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="4">
+        <v>0.98089201483743704</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="4">
+        <v>0.293501611779383</v>
+      </c>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0.98329209774725901</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N61" s="2">
+        <v>0.98604968436229801</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="18">
+        <v>4.3436922356910003E-3</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="4">
+        <v>4.6437314522779997E-3</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="4">
+        <v>1.9497077820217999E-2</v>
+      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K62" s="3">
+        <v>4.4503516209090004E-3</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N62" s="2">
+        <v>3.9458957978169996E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="18">
+        <v>6.3484742976839996E-3</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="4">
+        <v>6.8742617757579999E-3</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" s="4">
+        <v>3.6291835315035E-2</v>
+      </c>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K63" s="3">
+        <v>6.4340489494379999E-3</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N63">
+        <v>5.884276607973E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="23"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="10"/>
+      <c r="I65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L65" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="18">
+        <v>0.63718392240646504</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" s="4">
+        <v>0.57312637652195497</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H67" s="4">
+        <v>8.3048942076276E-2</v>
+      </c>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0.62510707337739502</v>
+      </c>
+      <c r="M67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N67" s="2">
+        <v>0.65702989164662895</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="18">
+        <v>3.072101196434E-3</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="4">
+        <v>3.2689449268779999E-3</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H68" s="4">
+        <v>4.3700549343979999E-3</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K68" s="3">
+        <v>3.1244743585590001E-3</v>
+      </c>
+      <c r="L68" s="17"/>
+      <c r="M68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N68" s="2">
+        <v>2.7564581830249999E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="18">
+        <v>9.3214706315860006E-3</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="4">
+        <v>9.9447711644580009E-3</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" s="4">
+        <v>1.249337393967E-2</v>
+      </c>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K69" s="3">
+        <v>9.4919078194020002E-3</v>
+      </c>
+      <c r="M69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N69" s="2">
+        <v>9.1318942553530007E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="23"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="10"/>
+      <c r="I71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K71" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="18">
+        <v>0.78260234216719105</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="4">
+        <v>0.76519579960408801</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H73" s="4">
+        <v>0.29731363232680902</v>
+      </c>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K73" s="3">
+        <v>0.778144143833993</v>
+      </c>
+      <c r="M73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N73" s="2">
+        <v>0.80113747638376198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="18">
+        <v>3.3863747565102E-2</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" s="4">
+        <v>3.5265063393780001E-2</v>
+      </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H74" s="4">
+        <v>6.4801597726184004E-2</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K74" s="3">
+        <v>3.4378532540865002E-2</v>
+      </c>
+      <c r="M74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N74" s="2">
+        <v>3.1488714686342997E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="18">
+        <v>5.5230315391926001E-2</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="4">
+        <v>5.720515491026E-2</v>
+      </c>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H75" s="4">
+        <v>9.5518651202831997E-2</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K75" s="3">
+        <v>5.5731106891128999E-2</v>
+      </c>
+      <c r="M75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N75" s="2">
+        <v>5.3075272429106E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C77" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59E890F-49BE-45EE-8E8F-F9CC2C8BF8BF}">
+  <dimension ref="A1:H57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.69481254169738804</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.864164651231076</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1.3647161408762E-2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1.0246652001194E-2</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2.2525171335086001E-2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="18">
+        <v>1.4339525504621E-2</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="F8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0.50220655193284902</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.52844073459788399</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2.5001974754238002E-2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1.7269844828825001E-2</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3.4251283982576E-2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="18">
+        <v>2.5561167111114998E-2</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="F14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.607117580723466</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.844379177287788</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2.4122857304778198</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0.17980206266523999</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="18">
+        <v>5.2710042781031303</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.237000320009776</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="19"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="F21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.97333648617217094</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0.98374923020516503</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5.0585177693840003E-3</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="18">
+        <v>4.3436922356910003E-3</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="4">
+        <v>7.6127248632249997E-3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="18">
+        <v>6.3484742976839996E-3</v>
+      </c>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="F27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="18">
+        <v>0.48360441899460899</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0.63718392240646504</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="4">
+        <v>2.629330426662E-3</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="18">
+        <v>3.072101196434E-3</v>
+      </c>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="18">
+        <v>5.3195656392579999E-3</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="18">
+        <v>9.3214706315860006E-3</v>
+      </c>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="F33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="23"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.78423777657081095</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="18">
+        <v>0.78260234216719105</v>
+      </c>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="4">
+        <v>3.3498570673979003E-2</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="18">
+        <v>3.3863747565102E-2</v>
+      </c>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="4">
+        <v>5.7968142520474997E-2</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="18">
+        <v>5.5230315391926001E-2</v>
+      </c>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="12"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add lateral plus longitudinal reconstruction until step1 and step 2
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
+++ b/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CE116-25CF-4EAC-97A4-DA56D5281118}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26982BA-8C8B-4FBE-88AE-A7414FA1C196}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
   </bookViews>
   <sheets>
     <sheet name="first_10_records_full_lateral" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="34">
   <si>
     <t>eMFIS(I/E)</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Backward</t>
+  </si>
+  <si>
+    <t>Laterl</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -628,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAED88D5-E873-5842-BA5A-48463FA2EFF5}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1730,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71B7EED-AC09-4997-9EF3-1224B488CEBF}">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3637,477 +3643,238 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59E890F-49BE-45EE-8E8F-F9CC2C8BF8BF}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="23"/>
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="18">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18">
         <v>0.69481254169738804</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="G4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="18">
         <v>0.864164651231076</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="18">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
         <v>1.3647161408762E-2</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="18">
         <v>1.0246652001194E-2</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="18">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18">
         <v>2.2525171335086001E-2</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="18">
         <v>1.4339525504621E-2</v>
       </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="F8" s="8" t="s">
+      <c r="C8" s="23"/>
+      <c r="G8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="18">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18">
         <v>0.50220655193284902</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="18">
+      <c r="G10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="18">
         <v>0.52844073459788399</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18">
         <v>2.5001974754238002E-2</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="18">
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="18">
         <v>1.7269844828825001E-2</v>
       </c>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="18">
         <v>3.4251283982576E-2</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="18">
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="18">
         <v>2.5561167111114998E-2</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="F14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
+      <c r="C13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.59643867657364902</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.607117580723466</v>
+      </c>
+      <c r="F14" s="18">
+        <v>0.81627222708007896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.58100547363065802</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2.4122857304778198</v>
+      </c>
+      <c r="F15" s="18">
+        <v>6.1839146302673002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
       </c>
       <c r="B16" s="18">
-        <v>0.607117580723466</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0.844379177287788</v>
-      </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="18">
-        <v>2.4122857304778198</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="18">
-        <v>0.17980206266523999</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="18">
+        <v>2.0735806301248099</v>
+      </c>
+      <c r="D16" s="18">
         <v>5.2710042781031303</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0.237000320009776</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="19"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="F21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0.97333648617217094</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0.98374923020516503</v>
-      </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="4">
-        <v>5.0585177693840003E-3</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" s="18">
-        <v>4.3436922356910003E-3</v>
-      </c>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="4">
-        <v>7.6127248632249997E-3</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="18">
-        <v>6.3484742976839996E-3</v>
-      </c>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="F27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="18">
-        <v>0.48360441899460899</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="18">
-        <v>0.63718392240646504</v>
-      </c>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="4">
-        <v>2.629330426662E-3</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G30" s="18">
-        <v>3.072101196434E-3</v>
-      </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="18">
-        <v>5.3195656392579999E-3</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="18">
-        <v>9.3214706315860006E-3</v>
-      </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="23"/>
-      <c r="F33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="4">
-        <v>0.78423777657081095</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G35" s="18">
-        <v>0.78260234216719105</v>
-      </c>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="4">
-        <v>3.3498570673979003E-2</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G36" s="18">
-        <v>3.3863747565102E-2</v>
-      </c>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="4">
-        <v>5.7968142520474997E-2</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37" s="18">
-        <v>5.5230315391926001E-2</v>
-      </c>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="3"/>
+      <c r="F16" s="18">
+        <v>0.107416555706096</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="12"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add data preparation for longitudinal and lateral prediction; Xie Chen
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
+++ b/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_predict_bank_failure\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26982BA-8C8B-4FBE-88AE-A7414FA1C196}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C48716-85B5-49EE-9B4B-46E51C1BC5B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
   </bookViews>
   <sheets>
     <sheet name="first_10_records_full_lateral" sheetId="1" r:id="rId1"/>
@@ -95,18 +95,6 @@
     <t>20% - 2</t>
   </si>
   <si>
-    <t>100% - 2485</t>
-  </si>
-  <si>
-    <t>Random-24% : 596</t>
-  </si>
-  <si>
-    <t>100% - 49338</t>
-  </si>
-  <si>
-    <t>Random-24% : 11841</t>
-  </si>
-  <si>
     <t>Backward_Prediction</t>
   </si>
   <si>
@@ -135,6 +123,18 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Random-24% : 481</t>
+  </si>
+  <si>
+    <t>100% - 2004</t>
+  </si>
+  <si>
+    <t>Random-24% : 9549</t>
+  </si>
+  <si>
+    <t>100% - 39789</t>
   </si>
 </sst>
 </file>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAED88D5-E873-5842-BA5A-48463FA2EFF5}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -805,13 +805,13 @@
         <v>10</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -961,13 +961,13 @@
         <v>10</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1117,13 +1117,13 @@
         <v>10</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K20" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1276,13 +1276,13 @@
         <v>10</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K27" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -1432,13 +1432,13 @@
         <v>10</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K33" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -1589,13 +1589,13 @@
         <v>10</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K39" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -1736,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71B7EED-AC09-4997-9EF3-1224B488CEBF}">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1750,7 +1750,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1772,13 +1772,13 @@
         <v>10</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -1927,13 +1927,13 @@
         <v>10</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -2082,13 +2082,13 @@
         <v>10</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -2241,13 +2241,13 @@
         <v>10</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K21" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -2396,13 +2396,13 @@
         <v>10</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K27" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -2552,13 +2552,13 @@
         <v>10</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K33" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -2694,7 +2694,7 @@
     </row>
     <row r="39" spans="1:14" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -2716,13 +2716,13 @@
         <v>10</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K40" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -2871,13 +2871,13 @@
         <v>10</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K46" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -3026,13 +3026,13 @@
         <v>10</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K52" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
@@ -3185,13 +3185,13 @@
         <v>10</v>
       </c>
       <c r="J59" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K59" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
@@ -3340,13 +3340,13 @@
         <v>10</v>
       </c>
       <c r="J65" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K65" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
@@ -3496,13 +3496,13 @@
         <v>10</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K71" s="20" t="s">
         <v>11</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
@@ -3653,10 +3653,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -3810,7 +3810,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" s="18">
         <v>0.59643867657364902</v>
@@ -3852,13 +3852,13 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Pretrain both lat and long systems again with 80% train and 20% unsessn data
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
+++ b/Experiment_Resulsts/Missing_Data_Reconstruction_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_predict_bank_failure\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C48716-85B5-49EE-9B4B-46E51C1BC5B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2198A82-71C2-4859-B0ED-00C85A2A7FA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0DF1D457-0958-2649-BAC9-ACE41436EACB}"/>
   </bookViews>
   <sheets>
     <sheet name="first_10_records_full_lateral" sheetId="1" r:id="rId1"/>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAED88D5-E873-5842-BA5A-48463FA2EFF5}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1736,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71B7EED-AC09-4997-9EF3-1224B488CEBF}">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>